<commit_message>
change column name in day_session_apes-table
</commit_message>
<xml_diff>
--- a/exp1/doc/day_session_apes.xlsx
+++ b/exp1/doc/day_session_apes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniela_schmidt/Documents/minerva/facet/analyses/facet_analysis_final/eyetracking-quality-devcomp/exp1/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DA4A0E-89EB-D74E-98AC-B865FB80CAA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625F5906-D749-FB4E-AA39-FB5700E3287B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35060" yWindow="600" windowWidth="32560" windowHeight="20640" xr2:uid="{2BE3EC54-E8B0-B94A-B892-7ED0FF4840D0}"/>
+    <workbookView xWindow="32140" yWindow="800" windowWidth="32560" windowHeight="20640" xr2:uid="{2BE3EC54-E8B0-B94A-B892-7ED0FF4840D0}"/>
   </bookViews>
   <sheets>
     <sheet name="A_Adults" sheetId="1" r:id="rId1"/>
@@ -137,9 +137,6 @@
     <t>date</t>
   </si>
   <si>
-    <t>group</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -147,6 +144,9 @@
   </si>
   <si>
     <t>group_id</t>
+  </si>
+  <si>
+    <t>species_group</t>
   </si>
 </sst>
 </file>
@@ -1024,18 +1024,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFF77F77-C255-1343-835D-E87AB6C95B62}">
   <dimension ref="A1:E178"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="10.83203125" style="9"/>
     <col min="4" max="4" width="10.83203125" style="2"/>
-    <col min="5" max="5" width="10.83203125" style="3"/>
+    <col min="5" max="5" width="14.33203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="32" t="s">
         <v>1</v>
@@ -1047,7 +1049,7 @@
         <v>22</v>
       </c>
       <c r="E1" s="34" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1064,7 +1066,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1081,7 +1083,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1098,7 +1100,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1115,7 +1117,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1132,7 +1134,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1149,7 +1151,7 @@
         <v>3</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1166,7 +1168,7 @@
         <v>4</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1183,7 +1185,7 @@
         <v>4</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1200,7 +1202,7 @@
         <v>5</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1217,7 +1219,7 @@
         <v>6</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1234,7 +1236,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1251,7 +1253,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1268,7 +1270,7 @@
         <v>2</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1285,7 +1287,7 @@
         <v>2</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1302,7 +1304,7 @@
         <v>3</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1319,7 +1321,7 @@
         <v>3</v>
       </c>
       <c r="E17" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1336,7 +1338,7 @@
         <v>4</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1353,7 +1355,7 @@
         <v>4</v>
       </c>
       <c r="E19" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1370,7 +1372,7 @@
         <v>5</v>
       </c>
       <c r="E20" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1387,7 +1389,7 @@
         <v>6</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1404,7 +1406,7 @@
         <v>7</v>
       </c>
       <c r="E22" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -1421,7 +1423,7 @@
         <v>1</v>
       </c>
       <c r="E23" s="36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1438,7 +1440,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1455,7 +1457,7 @@
         <v>2</v>
       </c>
       <c r="E25" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1472,7 +1474,7 @@
         <v>2</v>
       </c>
       <c r="E26" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1489,7 +1491,7 @@
         <v>3</v>
       </c>
       <c r="E27" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1506,7 +1508,7 @@
         <v>3</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1523,7 +1525,7 @@
         <v>4</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1540,7 +1542,7 @@
         <v>4</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -1557,7 +1559,7 @@
         <v>4</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1574,7 +1576,7 @@
         <v>5</v>
       </c>
       <c r="E32" s="42" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -1591,7 +1593,7 @@
         <v>1</v>
       </c>
       <c r="E33" s="37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -1608,7 +1610,7 @@
         <v>1</v>
       </c>
       <c r="E34" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -1625,7 +1627,7 @@
         <v>2</v>
       </c>
       <c r="E35" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1642,7 +1644,7 @@
         <v>2</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -1659,7 +1661,7 @@
         <v>3</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -1676,7 +1678,7 @@
         <v>3</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -1693,7 +1695,7 @@
         <v>4</v>
       </c>
       <c r="E39" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -1710,7 +1712,7 @@
         <v>4</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -1727,7 +1729,7 @@
         <v>5</v>
       </c>
       <c r="E41" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1744,7 +1746,7 @@
         <v>5</v>
       </c>
       <c r="E42" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -1761,7 +1763,7 @@
         <v>1</v>
       </c>
       <c r="E43" s="36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -1778,7 +1780,7 @@
         <v>1</v>
       </c>
       <c r="E44" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -1795,7 +1797,7 @@
         <v>2</v>
       </c>
       <c r="E45" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -1812,7 +1814,7 @@
         <v>2</v>
       </c>
       <c r="E46" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -1829,7 +1831,7 @@
         <v>3</v>
       </c>
       <c r="E47" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -1846,7 +1848,7 @@
         <v>3</v>
       </c>
       <c r="E48" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -1863,7 +1865,7 @@
         <v>4</v>
       </c>
       <c r="E49" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -1880,7 +1882,7 @@
         <v>4</v>
       </c>
       <c r="E50" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -1897,7 +1899,7 @@
         <v>5</v>
       </c>
       <c r="E51" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1914,7 +1916,7 @@
         <v>6</v>
       </c>
       <c r="E52" s="42" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -1931,7 +1933,7 @@
         <v>1</v>
       </c>
       <c r="E53" s="37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -1948,7 +1950,7 @@
         <v>1</v>
       </c>
       <c r="E54" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -1965,7 +1967,7 @@
         <v>2</v>
       </c>
       <c r="E55" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -1982,7 +1984,7 @@
         <v>2</v>
       </c>
       <c r="E56" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -1999,7 +2001,7 @@
         <v>3</v>
       </c>
       <c r="E57" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -2016,7 +2018,7 @@
         <v>3</v>
       </c>
       <c r="E58" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -2033,7 +2035,7 @@
         <v>4</v>
       </c>
       <c r="E59" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -2050,7 +2052,7 @@
         <v>4</v>
       </c>
       <c r="E60" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -2067,7 +2069,7 @@
         <v>5</v>
       </c>
       <c r="E61" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2084,7 +2086,7 @@
         <v>6</v>
       </c>
       <c r="E62" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -2101,7 +2103,7 @@
         <v>1</v>
       </c>
       <c r="E63" s="36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -2118,7 +2120,7 @@
         <v>1</v>
       </c>
       <c r="E64" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -2135,7 +2137,7 @@
         <v>2</v>
       </c>
       <c r="E65" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -2152,7 +2154,7 @@
         <v>2</v>
       </c>
       <c r="E66" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -2169,7 +2171,7 @@
         <v>3</v>
       </c>
       <c r="E67" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -2186,7 +2188,7 @@
         <v>3</v>
       </c>
       <c r="E68" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -2203,7 +2205,7 @@
         <v>4</v>
       </c>
       <c r="E69" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
@@ -2220,7 +2222,7 @@
         <v>4</v>
       </c>
       <c r="E70" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
@@ -2237,7 +2239,7 @@
         <v>5</v>
       </c>
       <c r="E71" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2254,7 +2256,7 @@
         <v>6</v>
       </c>
       <c r="E72" s="42" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
@@ -2271,7 +2273,7 @@
         <v>1</v>
       </c>
       <c r="E73" s="37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
@@ -2288,7 +2290,7 @@
         <v>1</v>
       </c>
       <c r="E74" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
@@ -2305,7 +2307,7 @@
         <v>2</v>
       </c>
       <c r="E75" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
@@ -2322,7 +2324,7 @@
         <v>2</v>
       </c>
       <c r="E76" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
@@ -2339,7 +2341,7 @@
         <v>3</v>
       </c>
       <c r="E77" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
@@ -2356,7 +2358,7 @@
         <v>3</v>
       </c>
       <c r="E78" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
@@ -2373,7 +2375,7 @@
         <v>4</v>
       </c>
       <c r="E79" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
@@ -2390,7 +2392,7 @@
         <v>4</v>
       </c>
       <c r="E80" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
@@ -2407,7 +2409,7 @@
         <v>5</v>
       </c>
       <c r="E81" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2424,7 +2426,7 @@
         <v>6</v>
       </c>
       <c r="E82" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -2441,7 +2443,7 @@
         <v>1</v>
       </c>
       <c r="E83" s="36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
@@ -2458,7 +2460,7 @@
         <v>1</v>
       </c>
       <c r="E84" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
@@ -2475,7 +2477,7 @@
         <v>2</v>
       </c>
       <c r="E85" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -2492,7 +2494,7 @@
         <v>2</v>
       </c>
       <c r="E86" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
@@ -2509,7 +2511,7 @@
         <v>3</v>
       </c>
       <c r="E87" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
@@ -2526,7 +2528,7 @@
         <v>3</v>
       </c>
       <c r="E88" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
@@ -2543,7 +2545,7 @@
         <v>4</v>
       </c>
       <c r="E89" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
@@ -2560,7 +2562,7 @@
         <v>4</v>
       </c>
       <c r="E90" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2577,7 +2579,7 @@
         <v>5</v>
       </c>
       <c r="E91" s="42" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -2594,7 +2596,7 @@
         <v>1</v>
       </c>
       <c r="E92" s="37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -2611,7 +2613,7 @@
         <v>1</v>
       </c>
       <c r="E93" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -2628,7 +2630,7 @@
         <v>2</v>
       </c>
       <c r="E94" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
@@ -2645,7 +2647,7 @@
         <v>2</v>
       </c>
       <c r="E95" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
@@ -2662,7 +2664,7 @@
         <v>3</v>
       </c>
       <c r="E96" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
@@ -2679,7 +2681,7 @@
         <v>3</v>
       </c>
       <c r="E97" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
@@ -2696,7 +2698,7 @@
         <v>4</v>
       </c>
       <c r="E98" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
@@ -2713,7 +2715,7 @@
         <v>4</v>
       </c>
       <c r="E99" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2730,7 +2732,7 @@
         <v>5</v>
       </c>
       <c r="E100" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
@@ -2747,7 +2749,7 @@
         <v>1</v>
       </c>
       <c r="E101" s="36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
@@ -2764,7 +2766,7 @@
         <v>1</v>
       </c>
       <c r="E102" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
@@ -2781,7 +2783,7 @@
         <v>2</v>
       </c>
       <c r="E103" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
@@ -2798,7 +2800,7 @@
         <v>2</v>
       </c>
       <c r="E104" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
@@ -2815,7 +2817,7 @@
         <v>3</v>
       </c>
       <c r="E105" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
@@ -2832,7 +2834,7 @@
         <v>3</v>
       </c>
       <c r="E106" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
@@ -2849,7 +2851,7 @@
         <v>4</v>
       </c>
       <c r="E107" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
@@ -2866,7 +2868,7 @@
         <v>4</v>
       </c>
       <c r="E108" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
@@ -2883,7 +2885,7 @@
         <v>5</v>
       </c>
       <c r="E109" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2900,7 +2902,7 @@
         <v>5</v>
       </c>
       <c r="E110" s="42" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
@@ -2917,7 +2919,7 @@
         <v>1</v>
       </c>
       <c r="E111" s="37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
@@ -2934,7 +2936,7 @@
         <v>1</v>
       </c>
       <c r="E112" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
@@ -2951,7 +2953,7 @@
         <v>2</v>
       </c>
       <c r="E113" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
@@ -2968,7 +2970,7 @@
         <v>2</v>
       </c>
       <c r="E114" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
@@ -2985,7 +2987,7 @@
         <v>3</v>
       </c>
       <c r="E115" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
@@ -3002,7 +3004,7 @@
         <v>3</v>
       </c>
       <c r="E116" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
@@ -3019,7 +3021,7 @@
         <v>4</v>
       </c>
       <c r="E117" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
@@ -3036,7 +3038,7 @@
         <v>4</v>
       </c>
       <c r="E118" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3053,7 +3055,7 @@
         <v>5</v>
       </c>
       <c r="E119" s="42" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
@@ -3070,7 +3072,7 @@
         <v>1</v>
       </c>
       <c r="E120" s="37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
@@ -3087,7 +3089,7 @@
         <v>1</v>
       </c>
       <c r="E121" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
@@ -3104,7 +3106,7 @@
         <v>2</v>
       </c>
       <c r="E122" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
@@ -3121,7 +3123,7 @@
         <v>2</v>
       </c>
       <c r="E123" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
@@ -3138,7 +3140,7 @@
         <v>3</v>
       </c>
       <c r="E124" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
@@ -3155,7 +3157,7 @@
         <v>3</v>
       </c>
       <c r="E125" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
@@ -3172,7 +3174,7 @@
         <v>4</v>
       </c>
       <c r="E126" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
@@ -3189,7 +3191,7 @@
         <v>4</v>
       </c>
       <c r="E127" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
@@ -3206,7 +3208,7 @@
         <v>5</v>
       </c>
       <c r="E128" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3223,7 +3225,7 @@
         <v>6</v>
       </c>
       <c r="E129" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
@@ -3240,7 +3242,7 @@
         <v>1</v>
       </c>
       <c r="E130" s="37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
@@ -3257,7 +3259,7 @@
         <v>1</v>
       </c>
       <c r="E131" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
@@ -3274,7 +3276,7 @@
         <v>2</v>
       </c>
       <c r="E132" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
@@ -3291,7 +3293,7 @@
         <v>2</v>
       </c>
       <c r="E133" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
@@ -3308,7 +3310,7 @@
         <v>3</v>
       </c>
       <c r="E134" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
@@ -3325,7 +3327,7 @@
         <v>3</v>
       </c>
       <c r="E135" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
@@ -3342,7 +3344,7 @@
         <v>4</v>
       </c>
       <c r="E136" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
@@ -3359,7 +3361,7 @@
         <v>4</v>
       </c>
       <c r="E137" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3376,7 +3378,7 @@
         <v>5</v>
       </c>
       <c r="E138" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
@@ -3393,7 +3395,7 @@
         <v>1</v>
       </c>
       <c r="E139" s="37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
@@ -3410,7 +3412,7 @@
         <v>1</v>
       </c>
       <c r="E140" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
@@ -3427,7 +3429,7 @@
         <v>2</v>
       </c>
       <c r="E141" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
@@ -3444,7 +3446,7 @@
         <v>2</v>
       </c>
       <c r="E142" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
@@ -3461,7 +3463,7 @@
         <v>3</v>
       </c>
       <c r="E143" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
@@ -3478,7 +3480,7 @@
         <v>3</v>
       </c>
       <c r="E144" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
@@ -3495,7 +3497,7 @@
         <v>4</v>
       </c>
       <c r="E145" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
@@ -3512,7 +3514,7 @@
         <v>4</v>
       </c>
       <c r="E146" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
@@ -3529,7 +3531,7 @@
         <v>5</v>
       </c>
       <c r="E147" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3546,7 +3548,7 @@
         <v>6</v>
       </c>
       <c r="E148" s="42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
@@ -3563,7 +3565,7 @@
         <v>1</v>
       </c>
       <c r="E149" s="37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
@@ -3580,7 +3582,7 @@
         <v>2</v>
       </c>
       <c r="E150" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
@@ -3597,7 +3599,7 @@
         <v>2</v>
       </c>
       <c r="E151" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
@@ -3614,7 +3616,7 @@
         <v>3</v>
       </c>
       <c r="E152" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
@@ -3631,7 +3633,7 @@
         <v>3</v>
       </c>
       <c r="E153" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
@@ -3648,7 +3650,7 @@
         <v>4</v>
       </c>
       <c r="E154" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
@@ -3665,7 +3667,7 @@
         <v>4</v>
       </c>
       <c r="E155" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
@@ -3682,7 +3684,7 @@
         <v>5</v>
       </c>
       <c r="E156" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
@@ -3699,7 +3701,7 @@
         <v>5</v>
       </c>
       <c r="E157" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
@@ -3716,7 +3718,7 @@
         <v>6</v>
       </c>
       <c r="E158" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3733,7 +3735,7 @@
         <v>7</v>
       </c>
       <c r="E159" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
@@ -3750,7 +3752,7 @@
         <v>1</v>
       </c>
       <c r="E160" s="36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
@@ -3767,7 +3769,7 @@
         <v>1</v>
       </c>
       <c r="E161" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
@@ -3784,7 +3786,7 @@
         <v>2</v>
       </c>
       <c r="E162" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
@@ -3801,7 +3803,7 @@
         <v>2</v>
       </c>
       <c r="E163" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
@@ -3818,7 +3820,7 @@
         <v>3</v>
       </c>
       <c r="E164" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
@@ -3835,7 +3837,7 @@
         <v>3</v>
       </c>
       <c r="E165" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
@@ -3852,7 +3854,7 @@
         <v>4</v>
       </c>
       <c r="E166" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
@@ -3869,7 +3871,7 @@
         <v>4</v>
       </c>
       <c r="E167" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
@@ -3886,7 +3888,7 @@
         <v>4</v>
       </c>
       <c r="E168" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="169" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3903,7 +3905,7 @@
         <v>5</v>
       </c>
       <c r="E169" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
@@ -3920,7 +3922,7 @@
         <v>1</v>
       </c>
       <c r="E170" s="37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
@@ -3937,7 +3939,7 @@
         <v>1</v>
       </c>
       <c r="E171" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
@@ -3954,7 +3956,7 @@
         <v>2</v>
       </c>
       <c r="E172" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
@@ -3971,7 +3973,7 @@
         <v>2</v>
       </c>
       <c r="E173" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
@@ -3988,7 +3990,7 @@
         <v>3</v>
       </c>
       <c r="E174" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
@@ -4005,7 +4007,7 @@
         <v>3</v>
       </c>
       <c r="E175" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
@@ -4022,7 +4024,7 @@
         <v>4</v>
       </c>
       <c r="E176" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
@@ -4039,7 +4041,7 @@
         <v>4</v>
       </c>
       <c r="E177" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="178" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4056,7 +4058,7 @@
         <v>5</v>
       </c>
       <c r="E178" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>